<commit_message>
updating examples for open-loop response time and constant-power DER injections
git-svn-id: https://svn.code.sf.net/p/electricdss/code/trunk@3536 d8739450-1e93-4ef4-a0af-c327d92816ff
</commit_message>
<xml_diff>
--- a/Version8/Distrib/Examples/ExpControl/Nantucket.xlsx
+++ b/Version8/Distrib/Examples/ExpControl/Nantucket.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Papers\2020_PESL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\OpenDSS\Version8\Distrib\Examples\ExpControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B70BC2A-BBB5-4111-9537-64587D751066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4727D8-DC23-4CDE-B074-9D0C12A58C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="951" yWindow="1551" windowWidth="19998" windowHeight="15240" activeTab="1" xr2:uid="{7F0E98FC-012E-4DF5-8696-4CB6DBA72C05}"/>
+    <workbookView xWindow="10329" yWindow="1217" windowWidth="17845" windowHeight="15240" activeTab="2" xr2:uid="{7F0E98FC-012E-4DF5-8696-4CB6DBA72C05}"/>
   </bookViews>
   <sheets>
     <sheet name="Hawaii" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="98">
   <si>
     <t>Condition</t>
   </si>
@@ -317,6 +317,24 @@
   <si>
     <t>opt pf</t>
   </si>
+  <si>
+    <t>Constant-Power</t>
+  </si>
+  <si>
+    <t>Im</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>VTcp</t>
+  </si>
+  <si>
+    <t>DSS d</t>
+  </si>
+  <si>
+    <t>(python NantucketRawSteps.py)</t>
+  </si>
 </sst>
 </file>
 
@@ -328,7 +346,7 @@
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +363,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -379,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -400,6 +426,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7563,10 +7592,667 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F4CA31-F04D-4F36-A538-838081015827}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P26"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="14.69140625" customWidth="1"/>
+    <col min="2" max="2" width="11.3046875" customWidth="1"/>
+    <col min="9" max="9" width="9.84375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5">
+        <f>C2*1000/SQRT(3)</f>
+        <v>7621.0235533030609</v>
+      </c>
+      <c r="C2">
+        <v>13.2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.8340000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B4/B3</f>
+        <v>2.3421487603305788</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <f>SQRT(B3*B3+B4*B4)</f>
+        <v>3.081502231055496</v>
+      </c>
+      <c r="C6" s="4">
+        <f>C2*C2/B6</f>
+        <v>56.543850023538091</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B2/B6</f>
+        <v>2473.1520478869356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <f>1/SQRT(1+1/B5/B5)</f>
+        <v>0.91968130720102714</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
+        <f>P9/$B$2</f>
+        <v>4.6228063635291736E-2</v>
+      </c>
+      <c r="C9" s="7">
+        <f>$D$2/3</f>
+        <v>2000000</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <f>$B$3*C9</f>
+        <v>2420000</v>
+      </c>
+      <c r="F9">
+        <f>$B$4*D9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <f>$B$4*C9</f>
+        <v>5668000</v>
+      </c>
+      <c r="H9">
+        <f>$B$3*D9</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>E9+F9</f>
+        <v>2420000</v>
+      </c>
+      <c r="J9">
+        <f>G9-H9</f>
+        <v>5668000</v>
+      </c>
+      <c r="K9">
+        <f>I9/$B$2</f>
+        <v>317.54264805429415</v>
+      </c>
+      <c r="L9">
+        <f>J9/$B$2</f>
+        <v>743.73211949245422</v>
+      </c>
+      <c r="M9" s="5">
+        <f>$B$2+K9</f>
+        <v>7938.5662013573547</v>
+      </c>
+      <c r="N9">
+        <f>L9</f>
+        <v>743.73211949245422</v>
+      </c>
+      <c r="O9">
+        <f>SQRT(M9*M9+N9*N9)</f>
+        <v>7973.328715091212</v>
+      </c>
+      <c r="P9" s="5">
+        <f>O9-B$2</f>
+        <v>352.30516178815105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10">
+        <f>P10/$B$2</f>
+        <v>-3.6710586338983192E-2</v>
+      </c>
+      <c r="C10" s="7">
+        <f>-$D$2/3</f>
+        <v>-2000000</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <f>$B$3*C10</f>
+        <v>-2420000</v>
+      </c>
+      <c r="F10">
+        <f>$B$4*D10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <f>$B$4*C10</f>
+        <v>-5668000</v>
+      </c>
+      <c r="H10">
+        <f>$B$3*D10</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>E10+F10</f>
+        <v>-2420000</v>
+      </c>
+      <c r="J10">
+        <f>G10-H10</f>
+        <v>-5668000</v>
+      </c>
+      <c r="K10">
+        <f>I10/$B$2</f>
+        <v>-317.54264805429415</v>
+      </c>
+      <c r="L10">
+        <f>J10/$B$2</f>
+        <v>-743.73211949245422</v>
+      </c>
+      <c r="M10" s="5">
+        <f>$B$2+K10</f>
+        <v>7303.4809052487672</v>
+      </c>
+      <c r="N10">
+        <f>L10</f>
+        <v>-743.73211949245422</v>
+      </c>
+      <c r="O10">
+        <f>SQRT(M10*M10+N10*N10)</f>
+        <v>7341.2513101581044</v>
+      </c>
+      <c r="P10" s="5">
+        <f>O10-B$2</f>
+        <v>-279.77224314495652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3">
+        <f>-(1/$B$8)*SQRT(1-$B$8*$B$8)</f>
+        <v>-0.42695836273817911</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10">
+        <f>P12/$B$2</f>
+        <v>6.6342039631844558E-3</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" ref="C12" si="0">$D$2/3</f>
+        <v>2000000</v>
+      </c>
+      <c r="D12" s="7">
+        <f>C12*$B$11</f>
+        <v>-853916.7254763582</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" ref="E12:E13" si="1">$B$3*C12</f>
+        <v>2420000</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F13" si="2">$B$4*D12</f>
+        <v>-2419999.9999999991</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" ref="G12:G13" si="3">$B$4*C12</f>
+        <v>5668000</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H13" si="4">$B$3*D12</f>
+        <v>-1033239.2378263935</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I13" si="5">E12+F12</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:J13" si="6">G12-H12</f>
+        <v>6701239.2378263939</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12:L13" si="7">I12/$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="7"/>
+        <v>879.30960860526147</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" ref="M12:M13" si="8">$B$2+K12</f>
+        <v>7621.0235533030609</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12:N13" si="9">L12</f>
+        <v>879.30960860526147</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O13" si="10">SQRT(M12*M12+N12*N12)</f>
+        <v>7671.5829779639062</v>
+      </c>
+      <c r="P12" s="5">
+        <f t="shared" ref="P12:P13" si="11">O12-B$2</f>
+        <v>50.559424660845252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10">
+        <f>P13/$B$2</f>
+        <v>6.6342039631844558E-3</v>
+      </c>
+      <c r="C13" s="7">
+        <f>-$D$2/3</f>
+        <v>-2000000</v>
+      </c>
+      <c r="D13" s="7">
+        <f>C13*$B$11</f>
+        <v>853916.7254763582</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="1"/>
+        <v>-2420000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>2419999.9999999991</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="3"/>
+        <v>-5668000</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>1033239.2378263935</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="6"/>
+        <v>-6701239.2378263939</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="7"/>
+        <v>-879.30960860526147</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="8"/>
+        <v>7621.0235533030609</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="9"/>
+        <v>-879.30960860526147</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="10"/>
+        <v>7671.5829779639062</v>
+      </c>
+      <c r="P13" s="5">
+        <f t="shared" si="11"/>
+        <v>50.559424660845252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4">
+        <f>2000000/B2</f>
+        <v>262.43194054073894</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2">
+        <f>B7/B15</f>
+        <v>9.4239750039230188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <f>B2</f>
+        <v>7621.0235533030609</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A20" s="11">
+        <f>B3</f>
+        <v>1.21</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="C20">
+        <f>$A$20*$A$20+A$21*$A$21</f>
+        <v>9.4956560000000003</v>
+      </c>
+      <c r="D20">
+        <f>2*$A$21*$A$19*$A$19</f>
+        <v>329197440.00000012</v>
+      </c>
+      <c r="E20" s="7">
+        <f>$B$20*$B$20*C20+2*$A$20*$A$19*$A$19*B20</f>
+        <v>319089824000000.06</v>
+      </c>
+      <c r="F20" s="7">
+        <f>(-D20+SQRT(D20*D20-4*C20*E20))/2/C20</f>
+        <v>-998027.36633974581</v>
+      </c>
+      <c r="G20" s="3">
+        <f>ABS(B20)/SQRT(B20*B20+F20*F20)</f>
+        <v>0.8947799269431097</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A21" s="11">
+        <f>B4</f>
+        <v>2.8340000000000001</v>
+      </c>
+      <c r="B21" s="7">
+        <v>-2000000</v>
+      </c>
+      <c r="C21">
+        <f>$A$20*$A$20+A$21*$A$21</f>
+        <v>9.4956560000000003</v>
+      </c>
+      <c r="D21">
+        <f>2*$A$21*$A$19*$A$19</f>
+        <v>329197440.00000012</v>
+      </c>
+      <c r="E21" s="7">
+        <f>$B$20*$B$20*C21+2*$A$20*$A$19*$A$19*B21</f>
+        <v>-243124576000000.06</v>
+      </c>
+      <c r="F21" s="7">
+        <f>(-D21+SQRT(D21*D21-4*C21*E21))/2/C21</f>
+        <v>723440.8219790702</v>
+      </c>
+      <c r="G21" s="3">
+        <f>ABS(B21)/SQRT(B21*B21+F21*F21)</f>
+        <v>0.94037072631073837</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="G22" s="3">
+        <f>AVERAGE(G20:G21)</f>
+        <v>0.91757532662692398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <f>B2</f>
+        <v>7621.0235533030609</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <f>B3</f>
+        <v>1.21</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <f>($A$25*C25-$A$26*B25)/$A$24</f>
+        <v>-743.73211949245422</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <f>-$A$24</f>
+        <v>-7621.0235533030609</v>
+      </c>
+      <c r="G25" s="7">
+        <f>D25*D25-$A$25*B25-$A$26*C25</f>
+        <v>-1866862.534435262</v>
+      </c>
+      <c r="H25" s="7">
+        <f>(-F25+SQRT(F25*F25-4*E25*G25))/2/E25</f>
+        <v>7858.5807650008228</v>
+      </c>
+      <c r="I25">
+        <f>SQRT(D25*D25+H25*H25)</f>
+        <v>7893.6955290665765</v>
+      </c>
+      <c r="J25" s="3">
+        <f>I25/$A$24-1</f>
+        <v>3.5778917865348259E-2</v>
+      </c>
+      <c r="K25">
+        <v>3.5799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <f>B4</f>
+        <v>2.8340000000000001</v>
+      </c>
+      <c r="B26" s="7">
+        <v>-2000000</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <f>($A$25*C26-$A$26*B26)/$A$24</f>
+        <v>743.73211949245422</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <f>-$A$24</f>
+        <v>-7621.0235533030609</v>
+      </c>
+      <c r="G26" s="7">
+        <f>D26*D26-$A$25*B26-$A$26*C26</f>
+        <v>2973137.465564738</v>
+      </c>
+      <c r="H26" s="7">
+        <f>(-F26+SQRT(F26*F26-4*E26*G26))/2/E26</f>
+        <v>7208.5792472052362</v>
+      </c>
+      <c r="I26">
+        <f>SQRT(D26*D26+H26*H26)</f>
+        <v>7246.844294505212</v>
+      </c>
+      <c r="J26" s="3">
+        <f>I26/$A$24-1</f>
+        <v>-4.9098294498207462E-2</v>
+      </c>
+      <c r="K26">
+        <v>-4.9099999999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571B5046-821A-4877-BBAD-1F65153958C2}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7609,7 +8295,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>1.21</v>
+        <v>1.744</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
@@ -7617,7 +8303,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.8340000000000001</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
@@ -7626,7 +8312,7 @@
       </c>
       <c r="B5" s="2">
         <f>B4/B3</f>
-        <v>2.3421487603305788</v>
+        <v>1.536697247706422</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
@@ -7635,11 +8321,11 @@
       </c>
       <c r="B6" s="2">
         <f>SQRT(B3*B3+B4*B4)</f>
-        <v>3.081502231055496</v>
+        <v>3.1974890148364858</v>
       </c>
       <c r="C6" s="4">
         <f>C2*C2/B6</f>
-        <v>56.543850023538091</v>
+        <v>54.492759534596971</v>
       </c>
       <c r="D6" t="s">
         <v>82</v>
@@ -7651,7 +8337,7 @@
       </c>
       <c r="B7" s="5">
         <f>B2/B6</f>
-        <v>2473.1520478869356</v>
+        <v>2383.4401050140236</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.4">
@@ -7660,7 +8346,7 @@
       </c>
       <c r="B8" s="3">
         <f>1/SQRT(1+1/B5/B5)</f>
-        <v>0.91968130720102714</v>
+        <v>0.83815768797474688</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -7711,7 +8397,7 @@
       </c>
       <c r="B9" s="10">
         <f>P9/$B$2</f>
-        <v>4.6228063635291736E-2</v>
+        <v>6.4064662405350123E-2</v>
       </c>
       <c r="C9" s="7">
         <f>$D$2/3</f>
@@ -7722,7 +8408,7 @@
       </c>
       <c r="E9" s="7">
         <f>$B$3*C9</f>
-        <v>2420000</v>
+        <v>3488000</v>
       </c>
       <c r="F9">
         <f>$B$4*D9</f>
@@ -7730,7 +8416,7 @@
       </c>
       <c r="G9" s="7">
         <f>$B$4*C9</f>
-        <v>5668000</v>
+        <v>5360000</v>
       </c>
       <c r="H9">
         <f>$B$3*D9</f>
@@ -7738,35 +8424,35 @@
       </c>
       <c r="I9">
         <f>E9+F9</f>
-        <v>2420000</v>
+        <v>3488000</v>
       </c>
       <c r="J9">
         <f>G9-H9</f>
-        <v>5668000</v>
+        <v>5360000</v>
       </c>
       <c r="K9">
         <f>I9/$B$2</f>
-        <v>317.54264805429415</v>
+        <v>457.68130430304876</v>
       </c>
       <c r="L9">
         <f>J9/$B$2</f>
-        <v>743.73211949245422</v>
+        <v>703.31760064918035</v>
       </c>
       <c r="M9" s="5">
         <f>$B$2+K9</f>
-        <v>7938.5662013573547</v>
+        <v>8078.7048576061097</v>
       </c>
       <c r="N9">
         <f>L9</f>
-        <v>743.73211949245422</v>
+        <v>703.31760064918035</v>
       </c>
       <c r="O9">
         <f>SQRT(M9*M9+N9*N9)</f>
-        <v>7973.328715091212</v>
+        <v>8109.2618544286433</v>
       </c>
       <c r="P9" s="5">
         <f>O9-B$2</f>
-        <v>352.30516178815105</v>
+        <v>488.23830112558244</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.4">
@@ -7775,7 +8461,7 @@
       </c>
       <c r="B10" s="10">
         <f>P10/$B$2</f>
-        <v>-3.6710586338983192E-2</v>
+        <v>-5.5535484994337928E-2</v>
       </c>
       <c r="C10" s="7">
         <f>-$D$2/3</f>
@@ -7786,7 +8472,7 @@
       </c>
       <c r="E10" s="7">
         <f>$B$3*C10</f>
-        <v>-2420000</v>
+        <v>-3488000</v>
       </c>
       <c r="F10">
         <f>$B$4*D10</f>
@@ -7794,7 +8480,7 @@
       </c>
       <c r="G10" s="7">
         <f>$B$4*C10</f>
-        <v>-5668000</v>
+        <v>-5360000</v>
       </c>
       <c r="H10">
         <f>$B$3*D10</f>
@@ -7802,35 +8488,35 @@
       </c>
       <c r="I10">
         <f>E10+F10</f>
-        <v>-2420000</v>
+        <v>-3488000</v>
       </c>
       <c r="J10">
         <f>G10-H10</f>
-        <v>-5668000</v>
+        <v>-5360000</v>
       </c>
       <c r="K10">
         <f>I10/$B$2</f>
-        <v>-317.54264805429415</v>
+        <v>-457.68130430304876</v>
       </c>
       <c r="L10">
         <f>J10/$B$2</f>
-        <v>-743.73211949245422</v>
+        <v>-703.31760064918035</v>
       </c>
       <c r="M10" s="5">
         <f>$B$2+K10</f>
-        <v>7303.4809052487672</v>
+        <v>7163.3422490000121</v>
       </c>
       <c r="N10">
         <f>L10</f>
-        <v>-743.73211949245422</v>
+        <v>-703.31760064918035</v>
       </c>
       <c r="O10">
         <f>SQRT(M10*M10+N10*N10)</f>
-        <v>7341.2513101581044</v>
+        <v>7197.7863141171028</v>
       </c>
       <c r="P10" s="5">
         <f>O10-B$2</f>
-        <v>-279.77224314495652</v>
+        <v>-423.23723918595806</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.4">
@@ -7839,7 +8525,7 @@
       </c>
       <c r="B11" s="3">
         <f>-(1/$B$8)*SQRT(1-$B$8*$B$8)</f>
-        <v>-0.42695836273817911</v>
+        <v>-0.65074626865671636</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.4">
@@ -7848,7 +8534,7 @@
       </c>
       <c r="B12" s="10">
         <f>P12/$B$2</f>
-        <v>6.6342039631844558E-3</v>
+        <v>8.5917524857318725E-3</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" ref="C12" si="0">$D$2/3</f>
@@ -7856,23 +8542,23 @@
       </c>
       <c r="D12" s="7">
         <f>C12*$B$11</f>
-        <v>-853916.7254763582</v>
+        <v>-1301492.5373134327</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" ref="E12:E13" si="1">$B$3*C12</f>
-        <v>2420000</v>
+        <v>3488000</v>
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F13" si="2">$B$4*D12</f>
-        <v>-2419999.9999999991</v>
+        <v>-3487999.9999999995</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" ref="G12:G13" si="3">$B$4*C12</f>
-        <v>5668000</v>
+        <v>5360000</v>
       </c>
       <c r="H12">
         <f t="shared" ref="H12:H13" si="4">$B$3*D12</f>
-        <v>-1033239.2378263935</v>
+        <v>-2269802.9850746267</v>
       </c>
       <c r="I12">
         <f t="shared" ref="I12:I13" si="5">E12+F12</f>
@@ -7880,7 +8566,7 @@
       </c>
       <c r="J12">
         <f t="shared" ref="J12:J13" si="6">G12-H12</f>
-        <v>6701239.2378263939</v>
+        <v>7629802.9850746263</v>
       </c>
       <c r="K12">
         <f t="shared" ref="K12:L13" si="7">I12/$B$2</f>
@@ -7888,7 +8574,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="7"/>
-        <v>879.30960860526147</v>
+        <v>1001.1520016583285</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" ref="M12:M13" si="8">$B$2+K12</f>
@@ -7896,15 +8582,15 @@
       </c>
       <c r="N12">
         <f t="shared" ref="N12:N13" si="9">L12</f>
-        <v>879.30960860526147</v>
+        <v>1001.1520016583285</v>
       </c>
       <c r="O12">
         <f t="shared" ref="O12:O13" si="10">SQRT(M12*M12+N12*N12)</f>
-        <v>7671.5829779639062</v>
+        <v>7686.5015013609736</v>
       </c>
       <c r="P12" s="5">
         <f t="shared" ref="P12:P13" si="11">O12-B$2</f>
-        <v>50.559424660845252</v>
+        <v>65.477948057912727</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
@@ -7913,7 +8599,7 @@
       </c>
       <c r="B13" s="10">
         <f>P13/$B$2</f>
-        <v>6.6342039631844558E-3</v>
+        <v>8.5917524857318725E-3</v>
       </c>
       <c r="C13" s="7">
         <f>-$D$2/3</f>
@@ -7921,23 +8607,23 @@
       </c>
       <c r="D13" s="7">
         <f>C13*$B$11</f>
-        <v>853916.7254763582</v>
+        <v>1301492.5373134327</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="1"/>
-        <v>-2420000</v>
+        <v>-3488000</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>2419999.9999999991</v>
+        <v>3487999.9999999995</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="3"/>
-        <v>-5668000</v>
+        <v>-5360000</v>
       </c>
       <c r="H13">
         <f t="shared" si="4"/>
-        <v>1033239.2378263935</v>
+        <v>2269802.9850746267</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
@@ -7945,7 +8631,7 @@
       </c>
       <c r="J13">
         <f t="shared" si="6"/>
-        <v>-6701239.2378263939</v>
+        <v>-7629802.9850746263</v>
       </c>
       <c r="K13">
         <f t="shared" si="7"/>
@@ -7953,7 +8639,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="7"/>
-        <v>-879.30960860526147</v>
+        <v>-1001.1520016583285</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="8"/>
@@ -7961,15 +8647,15 @@
       </c>
       <c r="N13">
         <f t="shared" si="9"/>
-        <v>-879.30960860526147</v>
+        <v>-1001.1520016583285</v>
       </c>
       <c r="O13">
         <f t="shared" si="10"/>
-        <v>7671.5829779639062</v>
+        <v>7686.5015013609736</v>
       </c>
       <c r="P13" s="5">
         <f t="shared" si="11"/>
-        <v>50.559424660845252</v>
+        <v>65.477948057912727</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.4">
@@ -7987,15 +8673,15 @@
       </c>
       <c r="B16" s="2">
         <f>B7/B15</f>
-        <v>9.4239750039230188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+        <v>9.0821265890994987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="5">
         <f>B2</f>
         <v>7621.0235533030609</v>
@@ -8019,68 +8705,196 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
         <f>B3</f>
-        <v>1.21</v>
+        <v>1.744</v>
       </c>
       <c r="B20" s="7">
         <v>2000000</v>
       </c>
       <c r="C20">
         <f>$A$20*$A$20+A$21*$A$21</f>
-        <v>9.4956560000000003</v>
+        <v>10.223936000000002</v>
       </c>
       <c r="D20">
         <f>2*$A$21*$A$19*$A$19</f>
-        <v>329197440.00000012</v>
+        <v>311308800.00000012</v>
       </c>
       <c r="E20" s="7">
         <f>$B$20*$B$20*C20+2*$A$20*$A$19*$A$19*B20</f>
-        <v>319089824000000.06</v>
+        <v>446061824000000.06</v>
       </c>
       <c r="F20" s="7">
         <f>(-D20+SQRT(D20*D20-4*C20*E20))/2/C20</f>
-        <v>-998027.36633974581</v>
+        <v>-1507493.8593806829</v>
       </c>
       <c r="G20" s="3">
         <f>ABS(B20)/SQRT(B20*B20+F20*F20)</f>
-        <v>0.8947799269431097</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+        <v>0.79856147425809587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
         <f>B4</f>
-        <v>2.8340000000000001</v>
+        <v>2.68</v>
       </c>
       <c r="B21" s="7">
         <v>-2000000</v>
       </c>
       <c r="C21">
         <f>$A$20*$A$20+A$21*$A$21</f>
-        <v>9.4956560000000003</v>
+        <v>10.223936000000002</v>
       </c>
       <c r="D21">
         <f>2*$A$21*$A$19*$A$19</f>
-        <v>329197440.00000012</v>
+        <v>311308800.00000012</v>
       </c>
       <c r="E21" s="7">
         <f>$B$20*$B$20*C21+2*$A$20*$A$19*$A$19*B21</f>
-        <v>-243124576000000.06</v>
+        <v>-364270336000000.06</v>
       </c>
       <c r="F21" s="7">
         <f>(-D21+SQRT(D21*D21-4*C21*E21))/2/C21</f>
-        <v>723440.8219790702</v>
+        <v>1128314.7254391636</v>
       </c>
       <c r="G21" s="3">
         <f>ABS(B21)/SQRT(B21*B21+F21*F21)</f>
-        <v>0.94037072631073837</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+        <v>0.87095804304018432</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G22" s="3">
         <f>AVERAGE(G20:G21)</f>
-        <v>0.91757532662692398</v>
+        <v>0.83475975864914009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <f>B2</f>
+        <v>7621.0235533030609</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <f>B3</f>
+        <v>1.744</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <f>($A$25*C25-$A$26*B25)/$A$24</f>
+        <v>-703.31760064918035</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <f>-$A$24</f>
+        <v>-7621.0235533030609</v>
+      </c>
+      <c r="G25" s="7">
+        <f>D25*D25-$A$25*B25-$A$26*C25</f>
+        <v>-2993344.3526170803</v>
+      </c>
+      <c r="H25" s="7">
+        <f>(-F25+SQRT(F25*F25-4*E25*G25))/2/E25</f>
+        <v>7995.4065605878104</v>
+      </c>
+      <c r="I25">
+        <f>SQRT(D25*D25+H25*H25)</f>
+        <v>8026.2806901125459</v>
+      </c>
+      <c r="J25" s="3">
+        <f>I25/$A$24-1</f>
+        <v>5.3176208415448345E-2</v>
+      </c>
+      <c r="K25">
+        <v>5.3199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <f>B4</f>
+        <v>2.68</v>
+      </c>
+      <c r="B26" s="7">
+        <v>-2000000</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <f>($A$25*C26-$A$26*B26)/$A$24</f>
+        <v>703.31760064918035</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <f>-$A$24</f>
+        <v>-7621.0235533030609</v>
+      </c>
+      <c r="G26" s="7">
+        <f>D26*D26-$A$25*B26-$A$26*C26</f>
+        <v>3982655.6473829197</v>
+      </c>
+      <c r="H26" s="7">
+        <f>(-F26+SQRT(F26*F26-4*E26*G26))/2/E26</f>
+        <v>7056.639370049098</v>
+      </c>
+      <c r="I26">
+        <f>SQRT(D26*D26+H26*H26)</f>
+        <v>7091.6017123291585</v>
+      </c>
+      <c r="J26" s="3">
+        <f>I26/$A$24-1</f>
+        <v>-6.9468600545715797E-2</v>
+      </c>
+      <c r="K26">
+        <v>-6.9500000000000006E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8089,12 +8903,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571B5046-821A-4877-BBAD-1F65153958C2}">
-  <dimension ref="A1:P22"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D88D56F-5866-4E1A-A9FD-BAB878AAC530}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8116,6 +8930,15 @@
       <c r="D1" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -8123,29 +8946,105 @@
       </c>
       <c r="B2" s="5">
         <f>C2*1000/SQRT(3)</f>
-        <v>7621.0235533030609</v>
-      </c>
-      <c r="C2">
-        <v>13.2</v>
+        <v>230.94010767585033</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.4</v>
       </c>
       <c r="D2" s="7">
         <v>6000000</v>
+      </c>
+      <c r="F2">
+        <v>7.5</v>
+      </c>
+      <c r="G2">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="H2">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.744</v>
+      <c r="B3" s="11">
+        <f>N3</f>
+        <v>1.228444444444445E-3</v>
+      </c>
+      <c r="C3" s="12">
+        <v>13.2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="14">
+        <f>C2</f>
+        <v>0.4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1.21</v>
+      </c>
+      <c r="L3">
+        <f>$G$5*K3</f>
+        <v>1.1111111111111115E-3</v>
+      </c>
+      <c r="M3">
+        <f>$G$4*$G$2</f>
+        <v>1.1733333333333334E-4</v>
+      </c>
+      <c r="N3">
+        <f>L3+M3</f>
+        <v>1.228444444444445E-3</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.68</v>
+      <c r="B4" s="11">
+        <f>N4</f>
+        <v>3.8226541781450881E-3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="14">
+        <f>G3*G3/F2</f>
+        <v>2.1333333333333336E-2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="13">
+        <v>2.8340000000000001</v>
+      </c>
+      <c r="L4">
+        <f>$G$5*K4</f>
+        <v>2.6023875114784215E-3</v>
+      </c>
+      <c r="M4">
+        <f>$G$4*$H$2</f>
+        <v>1.2202666666666668E-3</v>
+      </c>
+      <c r="N4">
+        <f>L4+M4</f>
+        <v>3.8226541781450881E-3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
@@ -8154,20 +9053,27 @@
       </c>
       <c r="B5" s="2">
         <f>B4/B3</f>
-        <v>1.536697247706422</v>
+        <v>3.1117843345971217</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <f>(C2/C3)^2</f>
+        <v>9.1827364554637313E-4</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="11">
         <f>SQRT(B3*B3+B4*B4)</f>
-        <v>3.1974890148364858</v>
+        <v>4.0151912431136477E-3</v>
       </c>
       <c r="C6" s="4">
         <f>C2*C2/B6</f>
-        <v>54.492759534596971</v>
+        <v>39.848662320733034</v>
       </c>
       <c r="D6" t="s">
         <v>82</v>
@@ -8179,7 +9085,7 @@
       </c>
       <c r="B7" s="5">
         <f>B2/B6</f>
-        <v>2383.4401050140236</v>
+        <v>57516.589794304273</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.4">
@@ -8188,7 +9094,7 @@
       </c>
       <c r="B8" s="3">
         <f>1/SQRT(1+1/B5/B5)</f>
-        <v>0.83815768797474688</v>
+        <v>0.95204784696151767</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -8239,7 +9145,7 @@
       </c>
       <c r="B9" s="10">
         <f>P9/$B$2</f>
-        <v>6.4064662405350123E-2</v>
+        <v>5.5843056208692919E-2</v>
       </c>
       <c r="C9" s="7">
         <f>$D$2/3</f>
@@ -8250,7 +9156,7 @@
       </c>
       <c r="E9" s="7">
         <f>$B$3*C9</f>
-        <v>3488000</v>
+        <v>2456.8888888888901</v>
       </c>
       <c r="F9">
         <f>$B$4*D9</f>
@@ -8258,7 +9164,7 @@
       </c>
       <c r="G9" s="7">
         <f>$B$4*C9</f>
-        <v>5360000</v>
+        <v>7645.3083562901766</v>
       </c>
       <c r="H9">
         <f>$B$3*D9</f>
@@ -8266,35 +9172,35 @@
       </c>
       <c r="I9">
         <f>E9+F9</f>
-        <v>3488000</v>
+        <v>2456.8888888888901</v>
       </c>
       <c r="J9">
         <f>G9-H9</f>
-        <v>5360000</v>
+        <v>7645.3083562901766</v>
       </c>
       <c r="K9">
         <f>I9/$B$2</f>
-        <v>457.68130430304876</v>
+        <v>10.638640960267509</v>
       </c>
       <c r="L9">
         <f>J9/$B$2</f>
-        <v>703.31760064918035</v>
+        <v>33.105156281563715</v>
       </c>
       <c r="M9" s="5">
         <f>$B$2+K9</f>
-        <v>8078.7048576061097</v>
+        <v>241.57874863611784</v>
       </c>
       <c r="N9">
         <f>L9</f>
-        <v>703.31760064918035</v>
+        <v>33.105156281563715</v>
       </c>
       <c r="O9">
         <f>SQRT(M9*M9+N9*N9)</f>
-        <v>8109.2618544286433</v>
+        <v>243.83650908963443</v>
       </c>
       <c r="P9" s="5">
         <f>O9-B$2</f>
-        <v>488.23830112558244</v>
+        <v>12.896401413784105</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.4">
@@ -8303,7 +9209,7 @@
       </c>
       <c r="B10" s="10">
         <f>P10/$B$2</f>
-        <v>-5.5535484994337928E-2</v>
+        <v>-3.5356079852546754E-2</v>
       </c>
       <c r="C10" s="7">
         <f>-$D$2/3</f>
@@ -8314,7 +9220,7 @@
       </c>
       <c r="E10" s="7">
         <f>$B$3*C10</f>
-        <v>-3488000</v>
+        <v>-2456.8888888888901</v>
       </c>
       <c r="F10">
         <f>$B$4*D10</f>
@@ -8322,7 +9228,7 @@
       </c>
       <c r="G10" s="7">
         <f>$B$4*C10</f>
-        <v>-5360000</v>
+        <v>-7645.3083562901766</v>
       </c>
       <c r="H10">
         <f>$B$3*D10</f>
@@ -8330,35 +9236,35 @@
       </c>
       <c r="I10">
         <f>E10+F10</f>
-        <v>-3488000</v>
+        <v>-2456.8888888888901</v>
       </c>
       <c r="J10">
         <f>G10-H10</f>
-        <v>-5360000</v>
+        <v>-7645.3083562901766</v>
       </c>
       <c r="K10">
         <f>I10/$B$2</f>
-        <v>-457.68130430304876</v>
+        <v>-10.638640960267509</v>
       </c>
       <c r="L10">
         <f>J10/$B$2</f>
-        <v>-703.31760064918035</v>
+        <v>-33.105156281563715</v>
       </c>
       <c r="M10" s="5">
         <f>$B$2+K10</f>
-        <v>7163.3422490000121</v>
+        <v>220.30146671558282</v>
       </c>
       <c r="N10">
         <f>L10</f>
-        <v>-703.31760064918035</v>
+        <v>-33.105156281563715</v>
       </c>
       <c r="O10">
         <f>SQRT(M10*M10+N10*N10)</f>
-        <v>7197.7863141171028</v>
+        <v>222.77497078770722</v>
       </c>
       <c r="P10" s="5">
         <f>O10-B$2</f>
-        <v>-423.23723918595806</v>
+        <v>-8.1651368881431097</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.4">
@@ -8367,7 +9273,7 @@
       </c>
       <c r="B11" s="3">
         <f>-(1/$B$8)*SQRT(1-$B$8*$B$8)</f>
-        <v>-0.65074626865671636</v>
+        <v>-0.32135903149903511</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.4">
@@ -8376,63 +9282,63 @@
       </c>
       <c r="B12" s="10">
         <f>P12/$B$2</f>
-        <v>8.5917524857318725E-3</v>
+        <v>1.2429019936634252E-2</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" ref="C12" si="0">$D$2/3</f>
+        <f>$D$2/3</f>
         <v>2000000</v>
       </c>
       <c r="D12" s="7">
         <f>C12*$B$11</f>
-        <v>-1301492.5373134327</v>
+        <v>-642718.06299807027</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" ref="E12:E13" si="1">$B$3*C12</f>
-        <v>3488000</v>
+        <f t="shared" ref="E12:E13" si="0">$B$3*C12</f>
+        <v>2456.8888888888901</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F13" si="2">$B$4*D12</f>
-        <v>-3487999.9999999995</v>
+        <f t="shared" ref="F12:F13" si="1">$B$4*D12</f>
+        <v>-2456.8888888888914</v>
       </c>
       <c r="G12" s="7">
-        <f t="shared" ref="G12:G13" si="3">$B$4*C12</f>
-        <v>5360000</v>
+        <f t="shared" ref="G12:G13" si="2">$B$4*C12</f>
+        <v>7645.3083562901766</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:H13" si="4">$B$3*D12</f>
-        <v>-2269802.9850746267</v>
+        <f t="shared" ref="H12:H13" si="3">$B$3*D12</f>
+        <v>-789.54343383407422</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I13" si="5">E12+F12</f>
+        <f t="shared" ref="I12:I13" si="4">E12+F12</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J13" si="6">G12-H12</f>
-        <v>7629802.9850746263</v>
+        <f t="shared" ref="J12:J13" si="5">G12-H12</f>
+        <v>8434.8517901242503</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:L13" si="7">I12/$B$2</f>
+        <f t="shared" ref="K12:L13" si="6">I12/$B$2</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="7"/>
-        <v>1001.1520016583285</v>
+        <f t="shared" si="6"/>
+        <v>36.523979637021242</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" ref="M12:M13" si="8">$B$2+K12</f>
-        <v>7621.0235533030609</v>
+        <f t="shared" ref="M12:M13" si="7">$B$2+K12</f>
+        <v>230.94010767585033</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N13" si="9">L12</f>
-        <v>1001.1520016583285</v>
+        <f t="shared" ref="N12:N13" si="8">L12</f>
+        <v>36.523979637021242</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O13" si="10">SQRT(M12*M12+N12*N12)</f>
-        <v>7686.5015013609736</v>
+        <f t="shared" ref="O12:O13" si="9">SQRT(M12*M12+N12*N12)</f>
+        <v>233.81046687832193</v>
       </c>
       <c r="P12" s="5">
-        <f t="shared" ref="P12:P13" si="11">O12-B$2</f>
-        <v>65.477948057912727</v>
+        <f t="shared" ref="P12:P13" si="10">O12-B$2</f>
+        <v>2.8703592024716045</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
@@ -8441,7 +9347,7 @@
       </c>
       <c r="B13" s="10">
         <f>P13/$B$2</f>
-        <v>8.5917524857318725E-3</v>
+        <v>1.2429019936634252E-2</v>
       </c>
       <c r="C13" s="7">
         <f>-$D$2/3</f>
@@ -8449,55 +9355,55 @@
       </c>
       <c r="D13" s="7">
         <f>C13*$B$11</f>
-        <v>1301492.5373134327</v>
+        <v>642718.06299807027</v>
       </c>
       <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>-2456.8888888888901</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="1"/>
-        <v>-3488000</v>
-      </c>
-      <c r="F13">
+        <v>2456.8888888888914</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="2"/>
-        <v>3487999.9999999995</v>
-      </c>
-      <c r="G13" s="7">
+        <v>-7645.3083562901766</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="3"/>
-        <v>-5360000</v>
-      </c>
-      <c r="H13">
+        <v>789.54343383407422</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="4"/>
-        <v>2269802.9850746267</v>
-      </c>
-      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="5"/>
+        <v>-8434.8517901242503</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <f t="shared" si="6"/>
-        <v>-7629802.9850746263</v>
-      </c>
-      <c r="K13">
+        <v>-36.523979637021242</v>
+      </c>
+      <c r="M13" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="7"/>
-        <v>-1001.1520016583285</v>
-      </c>
-      <c r="M13" s="5">
+        <v>230.94010767585033</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="8"/>
-        <v>7621.0235533030609</v>
-      </c>
-      <c r="N13">
+        <v>-36.523979637021242</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="9"/>
-        <v>-1001.1520016583285</v>
-      </c>
-      <c r="O13">
+        <v>233.81046687832193</v>
+      </c>
+      <c r="P13" s="5">
         <f t="shared" si="10"/>
-        <v>7686.5015013609736</v>
-      </c>
-      <c r="P13" s="5">
-        <f t="shared" si="11"/>
-        <v>65.477948057912727</v>
+        <v>2.8703592024716045</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.4">
@@ -8506,7 +9412,7 @@
       </c>
       <c r="B15" s="4">
         <f>2000000/B2</f>
-        <v>262.43194054073894</v>
+        <v>8660.2540378443864</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.4">
@@ -8515,634 +9421,15 @@
       </c>
       <c r="B16" s="2">
         <f>B7/B15</f>
-        <v>9.0821265890994987</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+        <v>6.6414437201221705</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="5">
-        <f>B2</f>
-        <v>7621.0235533030609</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="11">
-        <f>B3</f>
-        <v>1.744</v>
-      </c>
-      <c r="B20" s="7">
-        <v>2000000</v>
-      </c>
-      <c r="C20">
-        <f>$A$20*$A$20+A$21*$A$21</f>
-        <v>10.223936000000002</v>
-      </c>
-      <c r="D20">
-        <f>2*$A$21*$A$19*$A$19</f>
-        <v>311308800.00000012</v>
-      </c>
-      <c r="E20" s="7">
-        <f>$B$20*$B$20*C20+2*$A$20*$A$19*$A$19*B20</f>
-        <v>446061824000000.06</v>
-      </c>
-      <c r="F20" s="7">
-        <f>(-D20+SQRT(D20*D20-4*C20*E20))/2/C20</f>
-        <v>-1507493.8593806829</v>
-      </c>
-      <c r="G20" s="3">
-        <f>ABS(B20)/SQRT(B20*B20+F20*F20)</f>
-        <v>0.79856147425809587</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="11">
-        <f>B4</f>
-        <v>2.68</v>
-      </c>
-      <c r="B21" s="7">
-        <v>-2000000</v>
-      </c>
-      <c r="C21">
-        <f>$A$20*$A$20+A$21*$A$21</f>
-        <v>10.223936000000002</v>
-      </c>
-      <c r="D21">
-        <f>2*$A$21*$A$19*$A$19</f>
-        <v>311308800.00000012</v>
-      </c>
-      <c r="E21" s="7">
-        <f>$B$20*$B$20*C21+2*$A$20*$A$19*$A$19*B21</f>
-        <v>-364270336000000.06</v>
-      </c>
-      <c r="F21" s="7">
-        <f>(-D21+SQRT(D21*D21-4*C21*E21))/2/C21</f>
-        <v>1128314.7254391636</v>
-      </c>
-      <c r="G21" s="3">
-        <f>ABS(B21)/SQRT(B21*B21+F21*F21)</f>
-        <v>0.87095804304018432</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="G22" s="3">
-        <f>AVERAGE(G20:G21)</f>
-        <v>0.83475975864914009</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D88D56F-5866-4E1A-A9FD-BAB878AAC530}">
-  <dimension ref="A1:P22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="14.69140625" customWidth="1"/>
-    <col min="2" max="2" width="11.3046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5">
-        <f>C2*1000/SQRT(3)</f>
-        <v>230.94010767585033</v>
-      </c>
-      <c r="C2" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="D2" s="7">
-        <v>6000000</v>
-      </c>
-      <c r="F2">
-        <v>7.5</v>
-      </c>
-      <c r="G2">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="H2">
-        <v>5.7200000000000001E-2</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11">
-        <f>N3</f>
-        <v>1.228444444444445E-3</v>
-      </c>
-      <c r="C3" s="12">
-        <v>13.2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="14">
-        <v>0.4</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="13">
-        <v>1.21</v>
-      </c>
-      <c r="L3">
-        <f>$G$5*K3</f>
-        <v>1.1111111111111115E-3</v>
-      </c>
-      <c r="M3">
-        <f>$G$4*$G$2</f>
-        <v>1.1733333333333334E-4</v>
-      </c>
-      <c r="N3">
-        <f>L3+M3</f>
-        <v>1.228444444444445E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11">
-        <f>N4</f>
-        <v>3.8226541781450881E-3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="14">
-        <f>G3*G3/F2</f>
-        <v>2.1333333333333336E-2</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="13">
-        <v>2.8340000000000001</v>
-      </c>
-      <c r="L4">
-        <f>$G$5*K4</f>
-        <v>2.6023875114784215E-3</v>
-      </c>
-      <c r="M4">
-        <f>$G$4*$H$2</f>
-        <v>1.2202666666666668E-3</v>
-      </c>
-      <c r="N4">
-        <f>L4+M4</f>
-        <v>3.8226541781450881E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <f>B4/B3</f>
-        <v>3.1117843345971217</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5">
-        <f>(C2/C3)^2</f>
-        <v>9.1827364554637313E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="11">
-        <f>SQRT(B3*B3+B4*B4)</f>
-        <v>4.0151912431136477E-3</v>
-      </c>
-      <c r="C6" s="4">
-        <f>C2*C2/B6</f>
-        <v>39.848662320733034</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5">
-        <f>B2/B6</f>
-        <v>57516.589794304273</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3">
-        <f>1/SQRT(1+1/B5/B5)</f>
-        <v>0.95204784696151767</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="10">
-        <f>P9/$B$2</f>
-        <v>5.5843056208692919E-2</v>
-      </c>
-      <c r="C9" s="7">
-        <f>$D$2/3</f>
-        <v>2000000</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
-        <f>$B$3*C9</f>
-        <v>2456.8888888888901</v>
-      </c>
-      <c r="F9">
-        <f>$B$4*D9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
-        <f>$B$4*C9</f>
-        <v>7645.3083562901766</v>
-      </c>
-      <c r="H9">
-        <f>$B$3*D9</f>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f>E9+F9</f>
-        <v>2456.8888888888901</v>
-      </c>
-      <c r="J9">
-        <f>G9-H9</f>
-        <v>7645.3083562901766</v>
-      </c>
-      <c r="K9">
-        <f>I9/$B$2</f>
-        <v>10.638640960267509</v>
-      </c>
-      <c r="L9">
-        <f>J9/$B$2</f>
-        <v>33.105156281563715</v>
-      </c>
-      <c r="M9" s="5">
-        <f>$B$2+K9</f>
-        <v>241.57874863611784</v>
-      </c>
-      <c r="N9">
-        <f>L9</f>
-        <v>33.105156281563715</v>
-      </c>
-      <c r="O9">
-        <f>SQRT(M9*M9+N9*N9)</f>
-        <v>243.83650908963443</v>
-      </c>
-      <c r="P9" s="5">
-        <f>O9-B$2</f>
-        <v>12.896401413784105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="10">
-        <f>P10/$B$2</f>
-        <v>-3.5356079852546754E-2</v>
-      </c>
-      <c r="C10" s="7">
-        <f>-$D$2/3</f>
-        <v>-2000000</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
-        <f>$B$3*C10</f>
-        <v>-2456.8888888888901</v>
-      </c>
-      <c r="F10">
-        <f>$B$4*D10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
-        <f>$B$4*C10</f>
-        <v>-7645.3083562901766</v>
-      </c>
-      <c r="H10">
-        <f>$B$3*D10</f>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f>E10+F10</f>
-        <v>-2456.8888888888901</v>
-      </c>
-      <c r="J10">
-        <f>G10-H10</f>
-        <v>-7645.3083562901766</v>
-      </c>
-      <c r="K10">
-        <f>I10/$B$2</f>
-        <v>-10.638640960267509</v>
-      </c>
-      <c r="L10">
-        <f>J10/$B$2</f>
-        <v>-33.105156281563715</v>
-      </c>
-      <c r="M10" s="5">
-        <f>$B$2+K10</f>
-        <v>220.30146671558282</v>
-      </c>
-      <c r="N10">
-        <f>L10</f>
-        <v>-33.105156281563715</v>
-      </c>
-      <c r="O10">
-        <f>SQRT(M10*M10+N10*N10)</f>
-        <v>222.77497078770722</v>
-      </c>
-      <c r="P10" s="5">
-        <f>O10-B$2</f>
-        <v>-8.1651368881431097</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="3">
-        <f>-(1/$B$8)*SQRT(1-$B$8*$B$8)</f>
-        <v>-0.32135903149903511</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10">
-        <f>P12/$B$2</f>
-        <v>1.2429019936634252E-2</v>
-      </c>
-      <c r="C12" s="7">
-        <f>$D$2/3</f>
-        <v>2000000</v>
-      </c>
-      <c r="D12" s="7">
-        <f>C12*$B$11</f>
-        <v>-642718.06299807027</v>
-      </c>
-      <c r="E12" s="7">
-        <f t="shared" ref="E12:E13" si="0">$B$3*C12</f>
-        <v>2456.8888888888901</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ref="F12:F13" si="1">$B$4*D12</f>
-        <v>-2456.8888888888914</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" ref="G12:G13" si="2">$B$4*C12</f>
-        <v>7645.3083562901766</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ref="H12:H13" si="3">$B$3*D12</f>
-        <v>-789.54343383407422</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ref="I12:I13" si="4">E12+F12</f>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ref="J12:J13" si="5">G12-H12</f>
-        <v>8434.8517901242503</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ref="K12:L13" si="6">I12/$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="6"/>
-        <v>36.523979637021242</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" ref="M12:M13" si="7">$B$2+K12</f>
-        <v>230.94010767585033</v>
-      </c>
-      <c r="N12">
-        <f t="shared" ref="N12:N13" si="8">L12</f>
-        <v>36.523979637021242</v>
-      </c>
-      <c r="O12">
-        <f t="shared" ref="O12:O13" si="9">SQRT(M12*M12+N12*N12)</f>
-        <v>233.81046687832193</v>
-      </c>
-      <c r="P12" s="5">
-        <f t="shared" ref="P12:P13" si="10">O12-B$2</f>
-        <v>2.8703592024716045</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="10">
-        <f>P13/$B$2</f>
-        <v>1.2429019936634252E-2</v>
-      </c>
-      <c r="C13" s="7">
-        <f>-$D$2/3</f>
-        <v>-2000000</v>
-      </c>
-      <c r="D13" s="7">
-        <f>C13*$B$11</f>
-        <v>642718.06299807027</v>
-      </c>
-      <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>-2456.8888888888901</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>2456.8888888888914</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="2"/>
-        <v>-7645.3083562901766</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
-        <v>789.54343383407422</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>-8434.8517901242503</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="6"/>
-        <v>-36.523979637021242</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" si="7"/>
-        <v>230.94010767585033</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="8"/>
-        <v>-36.523979637021242</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="9"/>
-        <v>233.81046687832193</v>
-      </c>
-      <c r="P13" s="5">
-        <f t="shared" si="10"/>
-        <v>2.8703592024716045</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4">
-        <f>2000000/B2</f>
-        <v>8660.2540378443864</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2">
-        <f>B7/B15</f>
-        <v>6.6414437201221705</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="5">
         <f>B2</f>
         <v>230.94010767585033</v>
@@ -9166,7 +9453,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
         <f>B3</f>
         <v>1.228444444444445E-3</v>
@@ -9195,7 +9482,7 @@
         <v>0.92395305323883192</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
         <f>B4</f>
         <v>3.8226541781450881E-3</v>
@@ -9224,10 +9511,138 @@
         <v>0.97286865899309205</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G22" s="3">
         <f>AVERAGE(G20:G21)</f>
         <v>0.94841085611596199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <f>B2</f>
+        <v>230.94010767585033</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A25" s="11">
+        <f>B3</f>
+        <v>1.228444444444445E-3</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <f>($A$25*C25-$A$26*B25)/$A$24</f>
+        <v>-33.105156281563715</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <f>-$A$24</f>
+        <v>-230.94010767585033</v>
+      </c>
+      <c r="G25" s="7">
+        <f>D25*D25-$A$25*B25-$A$26*C25</f>
+        <v>-1360.9375164621326</v>
+      </c>
+      <c r="H25" s="7">
+        <f>(-F25+SQRT(F25*F25-4*E25*G25))/2/E25</f>
+        <v>236.6899814480152</v>
+      </c>
+      <c r="I25">
+        <f>SQRT(D25*D25+H25*H25)</f>
+        <v>238.99393023733583</v>
+      </c>
+      <c r="J25" s="3">
+        <f>I25/$A$24-1</f>
+        <v>3.4874074679093425E-2</v>
+      </c>
+      <c r="K25">
+        <v>3.49E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A26" s="11">
+        <f>B4</f>
+        <v>3.8226541781450881E-3</v>
+      </c>
+      <c r="B26" s="7">
+        <v>-2000000</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <f>($A$25*C26-$A$26*B26)/$A$24</f>
+        <v>33.105156281563715</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <f>-$A$24</f>
+        <v>-230.94010767585033</v>
+      </c>
+      <c r="G26" s="7">
+        <f>D26*D26-$A$25*B26-$A$26*C26</f>
+        <v>3552.8402613156477</v>
+      </c>
+      <c r="H26" s="7">
+        <f>(-F26+SQRT(F26*F26-4*E26*G26))/2/E26</f>
+        <v>214.36642926199056</v>
+      </c>
+      <c r="I26">
+        <f>SQRT(D26*D26+H26*H26)</f>
+        <v>216.90762404065646</v>
+      </c>
+      <c r="J26" s="3">
+        <f>I26/$A$24-1</f>
+        <v>-6.0762436531336506E-2</v>
+      </c>
+      <c r="K26">
+        <v>-6.08E-2</v>
       </c>
     </row>
   </sheetData>
@@ -9238,10 +9653,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04752002-1B45-4D28-B9E9-1A0171A57A1D}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G22"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9325,6 +9740,7 @@
         <v>81</v>
       </c>
       <c r="G3" s="14">
+        <f>C2</f>
         <v>0.4</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -9757,12 +10173,12 @@
         <v>6.5637239106154501</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="5">
         <f>B2</f>
         <v>230.94010767585033</v>
@@ -9786,7 +10202,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
         <f>B3</f>
         <v>1.7188025711662083E-3</v>
@@ -9815,7 +10231,7 @@
         <v>0.86533874272075995</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
         <f>B4</f>
         <v>3.681240036730947E-3</v>
@@ -9844,10 +10260,138 @@
         <v>0.93747965541205758</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G22" s="3">
         <f>AVERAGE(G20:G21)</f>
         <v>0.90140919906640882</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <f>B2</f>
+        <v>230.94010767585033</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A25" s="11">
+        <f>B3</f>
+        <v>1.7188025711662083E-3</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <f>($A$25*C25-$A$26*B25)/$A$24</f>
+        <v>-31.880473892373598</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <f>-$A$24</f>
+        <v>-230.94010767585033</v>
+      </c>
+      <c r="G25" s="7">
+        <f>D25*D25-$A$25*B25-$A$26*C25</f>
+        <v>-2421.2405267301019</v>
+      </c>
+      <c r="H25" s="7">
+        <f>(-F25+SQRT(F25*F25-4*E25*G25))/2/E25</f>
+        <v>240.98727918991995</v>
+      </c>
+      <c r="I25">
+        <f>SQRT(D25*D25+H25*H25)</f>
+        <v>243.08688435817086</v>
+      </c>
+      <c r="J25" s="3">
+        <f>I25/$A$24-1</f>
+        <v>5.2597085904930285E-2</v>
+      </c>
+      <c r="K25">
+        <v>5.2600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A26" s="11">
+        <f>B4</f>
+        <v>3.681240036730947E-3</v>
+      </c>
+      <c r="B26" s="7">
+        <v>-2000000</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <f>($A$25*C26-$A$26*B26)/$A$24</f>
+        <v>31.880473892373598</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <f>-$A$24</f>
+        <v>-230.94010767585033</v>
+      </c>
+      <c r="G26" s="7">
+        <f>D26*D26-$A$25*B26-$A$26*C26</f>
+        <v>4453.9697579347312</v>
+      </c>
+      <c r="H26" s="7">
+        <f>(-F26+SQRT(F26*F26-4*E26*G26))/2/E26</f>
+        <v>209.70042885255941</v>
+      </c>
+      <c r="I26">
+        <f>SQRT(D26*D26+H26*H26)</f>
+        <v>212.10995845680995</v>
+      </c>
+      <c r="J26" s="3">
+        <f>I26/$A$24-1</f>
+        <v>-8.1536937903703421E-2</v>
+      </c>
+      <c r="K26">
+        <v>-8.1500000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>